<commit_message>
Remove markdown report and add slide assets and scripts
Deleted FINAL_INTEGRATED_REPORT.md and added new slide images, report assets, and export_slide_plots.py script. Updated FINAL_INTEGRATED_REPORT.tex and several analysis outputs to reflect new figures and results. These changes support updated reporting and presentation workflows.
</commit_message>
<xml_diff>
--- a/final_analysis/Analysis long finals-.xlsx
+++ b/final_analysis/Analysis long finals-.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duccioo/Desktop/ai_memory_experiment/final_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1664686A-D67E-BE4C-8A54-B2E029B1EFB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D364E655-95A9-E741-B108-B3D2A2E77737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -589,13 +589,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="119" workbookViewId="0">
-      <selection activeCell="N68" sqref="N68"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="119" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="19" style="2"/>
+    <col min="1" max="15" width="19" style="2"/>
+    <col min="16" max="16" width="23.83203125" style="2" customWidth="1"/>
+    <col min="17" max="16384" width="19" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
@@ -748,10 +750,10 @@
         <v>4</v>
       </c>
       <c r="M3" s="2">
-        <v>10.64</v>
+        <v>8.6</v>
       </c>
       <c r="N3" s="2">
-        <v>532.91</v>
+        <v>102.5</v>
       </c>
       <c r="O3" s="2">
         <v>7</v>
@@ -1255,7 +1257,7 @@
         <v>8.0399999999999991</v>
       </c>
       <c r="N12" s="2">
-        <v>313.77999999999997</v>
+        <v>103.6</v>
       </c>
       <c r="O12" s="2">
         <v>7</v>
@@ -1420,10 +1422,10 @@
         <v>5</v>
       </c>
       <c r="M15" s="2">
-        <v>13.2</v>
+        <v>6.87</v>
       </c>
       <c r="N15" s="2">
-        <v>379.5</v>
+        <v>105.3</v>
       </c>
       <c r="O15" s="2">
         <v>6</v>
@@ -1588,7 +1590,7 @@
         <v>5</v>
       </c>
       <c r="M18" s="2">
-        <v>8.49</v>
+        <v>4.62</v>
       </c>
       <c r="N18" s="2">
         <v>232.48</v>
@@ -1703,7 +1705,7 @@
         <v>6.91</v>
       </c>
       <c r="N20" s="2">
-        <v>362.08</v>
+        <v>103.5</v>
       </c>
       <c r="O20" s="2">
         <v>5</v>
@@ -1924,7 +1926,7 @@
         <v>2</v>
       </c>
       <c r="M24" s="2">
-        <v>11.62</v>
+        <v>10.54</v>
       </c>
       <c r="N24" s="2">
         <v>64.95</v>
@@ -2092,7 +2094,7 @@
         <v>5</v>
       </c>
       <c r="M27" s="2">
-        <v>11.72</v>
+        <v>9.9600000000000009</v>
       </c>
       <c r="N27" s="2">
         <v>105.68</v>
@@ -2260,7 +2262,7 @@
         <v>4</v>
       </c>
       <c r="M30" s="2">
-        <v>5.34</v>
+        <v>4.9800000000000004</v>
       </c>
       <c r="N30" s="2">
         <v>21.84</v>
@@ -2596,7 +2598,7 @@
         <v>3</v>
       </c>
       <c r="M36" s="2">
-        <v>10.72</v>
+        <v>9.69</v>
       </c>
       <c r="N36" s="2">
         <v>61.99</v>
@@ -2764,7 +2766,7 @@
         <v>3</v>
       </c>
       <c r="M39" s="2">
-        <v>6.96</v>
+        <v>5.44</v>
       </c>
       <c r="N39" s="2">
         <v>91.28</v>
@@ -2932,7 +2934,7 @@
         <v>2</v>
       </c>
       <c r="M42" s="2">
-        <v>3.31</v>
+        <v>2.88</v>
       </c>
       <c r="N42" s="2">
         <v>25.67</v>
@@ -3268,7 +3270,7 @@
         <v>4</v>
       </c>
       <c r="M48" s="2">
-        <v>10.19</v>
+        <v>8.33</v>
       </c>
       <c r="N48" s="2">
         <v>111.65</v>
@@ -3436,7 +3438,7 @@
         <v>1</v>
       </c>
       <c r="M51" s="2">
-        <v>9.33</v>
+        <v>5.68</v>
       </c>
       <c r="N51" s="2">
         <v>219.1</v>
@@ -3604,7 +3606,7 @@
         <v>4</v>
       </c>
       <c r="M54" s="2">
-        <v>15</v>
+        <v>13.44</v>
       </c>
       <c r="N54" s="2">
         <v>93.74</v>
@@ -3772,7 +3774,7 @@
         <v>5</v>
       </c>
       <c r="M57" s="2">
-        <v>4.5999999999999996</v>
+        <v>3.57</v>
       </c>
       <c r="N57" s="2">
         <v>61.58</v>
@@ -3940,7 +3942,7 @@
         <v>5</v>
       </c>
       <c r="M60" s="2">
-        <v>5.6</v>
+        <v>5</v>
       </c>
       <c r="N60" s="2">
         <v>36.229999999999997</v>
@@ -4108,7 +4110,7 @@
         <v>5</v>
       </c>
       <c r="M63" s="2">
-        <v>5.73</v>
+        <v>3.73</v>
       </c>
       <c r="N63" s="2">
         <v>110.9032</v>
@@ -4276,7 +4278,7 @@
         <v>2</v>
       </c>
       <c r="M66" s="2">
-        <v>14.39</v>
+        <v>11.83</v>
       </c>
       <c r="N66" s="2">
         <v>153.65</v>
@@ -4444,7 +4446,7 @@
         <v>6</v>
       </c>
       <c r="M69" s="2">
-        <v>8.9700000000000006</v>
+        <v>7.09</v>
       </c>
       <c r="N69" s="2">
         <v>113.16</v>
@@ -4612,7 +4614,7 @@
         <v>6</v>
       </c>
       <c r="M72" s="2">
-        <v>12.02</v>
+        <v>9.3800000000000008</v>
       </c>
       <c r="N72" s="2">
         <v>135.82</v>

</xml_diff>